<commit_message>
feat: Improve GimmeMotifs process
</commit_message>
<xml_diff>
--- a/scATAC/data/sample.xlsx
+++ b/scATAC/data/sample.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28827"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="29127"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\software\JetBrains\JetBrains\PyCharm\PyCharmwp\scvdb_reproducibility\scATAC\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6149B740-C46A-4C7C-B743-372030CCE874}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{900D9077-D7D4-41D3-B6FB-AF0E6AFE558F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7326" uniqueCount="1082">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7326" uniqueCount="1088">
   <si>
     <t>gse_id</t>
   </si>
@@ -3595,6 +3595,30 @@
   </si>
   <si>
     <t>Skin</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>sample_id_19</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>sample_id_20</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>sample_id_25</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>sample_id_26</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>sample_id_27</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>sample_id_28</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -3981,8 +4005,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:AH363"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="I2" sqref="I2"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="F35" sqref="F35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -4846,7 +4870,7 @@
     </row>
     <row r="20" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A20" s="1" t="s">
-        <v>73</v>
+        <v>1082</v>
       </c>
       <c r="B20" s="1">
         <v>1</v>
@@ -4890,7 +4914,7 @@
     </row>
     <row r="21" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A21" s="1" t="s">
-        <v>76</v>
+        <v>1083</v>
       </c>
       <c r="B21" s="1">
         <v>1</v>
@@ -5110,7 +5134,7 @@
     </row>
     <row r="26" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A26" s="1" t="s">
-        <v>143</v>
+        <v>1084</v>
       </c>
       <c r="B26" s="1">
         <v>1</v>
@@ -5154,7 +5178,7 @@
     </row>
     <row r="27" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A27" s="1" t="s">
-        <v>144</v>
+        <v>1085</v>
       </c>
       <c r="B27" s="1">
         <v>0</v>
@@ -5198,7 +5222,7 @@
     </row>
     <row r="28" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A28" s="1" t="s">
-        <v>145</v>
+        <v>1086</v>
       </c>
       <c r="B28" s="1">
         <v>0</v>
@@ -5242,7 +5266,7 @@
     </row>
     <row r="29" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A29" s="1" t="s">
-        <v>146</v>
+        <v>1087</v>
       </c>
       <c r="B29" s="1">
         <v>0</v>
@@ -20051,8 +20075,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8787CBC2-21FC-4588-B485-8742706CBCF3}">
   <dimension ref="A1:O184"/>
   <sheetViews>
-    <sheetView topLeftCell="C1" workbookViewId="0">
-      <selection activeCell="H2" sqref="H2"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E30" sqref="E30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>

</xml_diff>

<commit_message>
feat: Improve chromVAR 和 GimmeMotifs process
</commit_message>
<xml_diff>
--- a/scATAC/data/sample.xlsx
+++ b/scATAC/data/sample.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\software\JetBrains\JetBrains\PyCharm\PyCharmwp\scvdb_reproducibility\scATAC\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{900D9077-D7D4-41D3-B6FB-AF0E6AFE558F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8489991A-96C4-4632-AE25-69F5D909EB9D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -4005,7 +4005,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:AH363"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
+    <sheetView topLeftCell="A325" zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="F35" sqref="F35"/>
     </sheetView>
   </sheetViews>
@@ -20075,8 +20075,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8787CBC2-21FC-4588-B485-8742706CBCF3}">
   <dimension ref="A1:O184"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E30" sqref="E30"/>
+    <sheetView tabSelected="1" topLeftCell="A85" workbookViewId="0">
+      <selection activeCell="E104" sqref="E104"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -20084,12 +20084,12 @@
     <col min="1" max="1" width="13.75" style="1" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="14.125" style="1" customWidth="1"/>
     <col min="3" max="3" width="9.625" style="1" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="9.625" style="1" customWidth="1"/>
-    <col min="5" max="5" width="9.5" style="1" customWidth="1"/>
-    <col min="6" max="6" width="8.25" style="1" customWidth="1"/>
-    <col min="7" max="7" width="9" style="1"/>
-    <col min="8" max="8" width="8.875" style="1" customWidth="1"/>
-    <col min="9" max="9" width="8.25" style="1" customWidth="1"/>
+    <col min="4" max="4" width="28.375" style="1" customWidth="1"/>
+    <col min="5" max="5" width="25.75" style="1" customWidth="1"/>
+    <col min="6" max="6" width="17.5" style="1" customWidth="1"/>
+    <col min="7" max="7" width="15.625" style="1" customWidth="1"/>
+    <col min="8" max="8" width="12.25" style="1" customWidth="1"/>
+    <col min="9" max="9" width="16.625" style="1" customWidth="1"/>
     <col min="10" max="10" width="9" style="1"/>
     <col min="11" max="11" width="41.75" style="1" customWidth="1"/>
     <col min="12" max="12" width="49.875" style="1" customWidth="1"/>

</xml_diff>

<commit_message>
feat: Improve sample process
</commit_message>
<xml_diff>
--- a/scATAC/data/sample.xlsx
+++ b/scATAC/data/sample.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\software\JetBrains\JetBrains\PyCharm\PyCharmwp\scvdb_reproducibility\scATAC\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8489991A-96C4-4632-AE25-69F5D909EB9D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{87B948AA-CBA6-4457-A631-132469C75655}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7326" uniqueCount="1088">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7329" uniqueCount="1091">
   <si>
     <t>gse_id</t>
   </si>
@@ -3619,6 +3619,18 @@
   </si>
   <si>
     <t>sample_id_28</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>f_sex</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>f_time</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>f_drug</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -20073,33 +20085,33 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8787CBC2-21FC-4588-B485-8742706CBCF3}">
-  <dimension ref="A1:O184"/>
+  <dimension ref="A1:R184"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A85" workbookViewId="0">
-      <selection activeCell="E104" sqref="E104"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E24" sqref="E24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="13.75" style="1" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="14.125" style="1" customWidth="1"/>
+    <col min="2" max="2" width="10.875" style="1" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="9.625" style="1" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="28.375" style="1" customWidth="1"/>
-    <col min="5" max="5" width="25.75" style="1" customWidth="1"/>
-    <col min="6" max="6" width="17.5" style="1" customWidth="1"/>
-    <col min="7" max="7" width="15.625" style="1" customWidth="1"/>
-    <col min="8" max="8" width="12.25" style="1" customWidth="1"/>
-    <col min="9" max="9" width="16.625" style="1" customWidth="1"/>
+    <col min="4" max="4" width="15.75" style="1" customWidth="1"/>
+    <col min="5" max="5" width="25.5" style="1" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="10.875" style="1" customWidth="1"/>
+    <col min="7" max="7" width="10.625" style="1" customWidth="1"/>
+    <col min="8" max="8" width="9.5" style="1" customWidth="1"/>
+    <col min="9" max="9" width="10" style="1" customWidth="1"/>
     <col min="10" max="10" width="9" style="1"/>
-    <col min="11" max="11" width="41.75" style="1" customWidth="1"/>
-    <col min="12" max="12" width="49.875" style="1" customWidth="1"/>
+    <col min="11" max="11" width="11.25" style="1" customWidth="1"/>
+    <col min="12" max="12" width="9.5" style="1" customWidth="1"/>
     <col min="13" max="13" width="9.125" style="1" customWidth="1"/>
-    <col min="14" max="14" width="8.375" style="1" customWidth="1"/>
-    <col min="15" max="15" width="8.875" style="1" customWidth="1"/>
+    <col min="14" max="14" width="11.375" style="1" customWidth="1"/>
+    <col min="15" max="15" width="12.875" style="1" customWidth="1"/>
     <col min="16" max="16384" width="9" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>1067</v>
       </c>
@@ -20145,8 +20157,17 @@
       <c r="O1" s="1" t="s">
         <v>1071</v>
       </c>
-    </row>
-    <row r="2" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="P1" s="1" t="s">
+        <v>1089</v>
+      </c>
+      <c r="Q1" s="1" t="s">
+        <v>1088</v>
+      </c>
+      <c r="R1" s="1" t="s">
+        <v>1090</v>
+      </c>
+    </row>
+    <row r="2" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A2" s="1" t="s">
         <v>80</v>
       </c>
@@ -20192,8 +20213,17 @@
       <c r="O2" s="1" t="s">
         <v>1073</v>
       </c>
-    </row>
-    <row r="3" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="P2" s="1">
+        <v>0</v>
+      </c>
+      <c r="Q2" s="1">
+        <v>0</v>
+      </c>
+      <c r="R2" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A3" s="1" t="s">
         <v>10</v>
       </c>
@@ -20239,8 +20269,17 @@
       <c r="O3" s="1" t="s">
         <v>1074</v>
       </c>
-    </row>
-    <row r="4" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="P3" s="1">
+        <v>0</v>
+      </c>
+      <c r="Q3" s="1">
+        <v>0</v>
+      </c>
+      <c r="R3" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A4" s="1" t="s">
         <v>11</v>
       </c>
@@ -20286,8 +20325,17 @@
       <c r="O4" s="1" t="s">
         <v>1074</v>
       </c>
-    </row>
-    <row r="5" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="P4" s="1">
+        <v>0</v>
+      </c>
+      <c r="Q4" s="1">
+        <v>0</v>
+      </c>
+      <c r="R4" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A5" s="1" t="s">
         <v>16</v>
       </c>
@@ -20333,8 +20381,17 @@
       <c r="O5" s="1" t="s">
         <v>1073</v>
       </c>
-    </row>
-    <row r="6" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="P5" s="1">
+        <v>0</v>
+      </c>
+      <c r="Q5" s="1">
+        <v>0</v>
+      </c>
+      <c r="R5" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A6" s="1" t="s">
         <v>19</v>
       </c>
@@ -20380,8 +20437,17 @@
       <c r="O6" s="1" t="s">
         <v>1074</v>
       </c>
-    </row>
-    <row r="7" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="P6" s="1">
+        <v>1</v>
+      </c>
+      <c r="Q6" s="1">
+        <v>1</v>
+      </c>
+      <c r="R6" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A7" s="1" t="s">
         <v>23</v>
       </c>
@@ -20427,8 +20493,17 @@
       <c r="O7" s="1" t="s">
         <v>1074</v>
       </c>
-    </row>
-    <row r="8" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="P7" s="1">
+        <v>1</v>
+      </c>
+      <c r="Q7" s="1">
+        <v>1</v>
+      </c>
+      <c r="R7" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A8" s="1" t="s">
         <v>27</v>
       </c>
@@ -20474,8 +20549,17 @@
       <c r="O8" s="1" t="s">
         <v>1074</v>
       </c>
-    </row>
-    <row r="9" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="P8" s="1">
+        <v>1</v>
+      </c>
+      <c r="Q8" s="1">
+        <v>1</v>
+      </c>
+      <c r="R8" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A9" s="1" t="s">
         <v>31</v>
       </c>
@@ -20521,8 +20605,17 @@
       <c r="O9" s="1" t="s">
         <v>1074</v>
       </c>
-    </row>
-    <row r="10" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="P9" s="1">
+        <v>1</v>
+      </c>
+      <c r="Q9" s="1">
+        <v>1</v>
+      </c>
+      <c r="R9" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A10" s="1" t="s">
         <v>35</v>
       </c>
@@ -20568,8 +20661,17 @@
       <c r="O10" s="1" t="s">
         <v>1074</v>
       </c>
-    </row>
-    <row r="11" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="P10" s="1">
+        <v>1</v>
+      </c>
+      <c r="Q10" s="1">
+        <v>1</v>
+      </c>
+      <c r="R10" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A11" s="1" t="s">
         <v>39</v>
       </c>
@@ -20615,8 +20717,17 @@
       <c r="O11" s="1" t="s">
         <v>1074</v>
       </c>
-    </row>
-    <row r="12" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="P11" s="1">
+        <v>1</v>
+      </c>
+      <c r="Q11" s="1">
+        <v>1</v>
+      </c>
+      <c r="R11" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A12" s="1" t="s">
         <v>46</v>
       </c>
@@ -20662,8 +20773,17 @@
       <c r="O12" s="1" t="s">
         <v>1074</v>
       </c>
-    </row>
-    <row r="13" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="P12" s="1">
+        <v>1</v>
+      </c>
+      <c r="Q12" s="1">
+        <v>1</v>
+      </c>
+      <c r="R12" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A13" s="1" t="s">
         <v>50</v>
       </c>
@@ -20709,8 +20829,17 @@
       <c r="O13" s="1" t="s">
         <v>1074</v>
       </c>
-    </row>
-    <row r="14" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="P13" s="1">
+        <v>1</v>
+      </c>
+      <c r="Q13" s="1">
+        <v>1</v>
+      </c>
+      <c r="R13" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="14" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A14" s="1" t="s">
         <v>53</v>
       </c>
@@ -20756,8 +20885,17 @@
       <c r="O14" s="1" t="s">
         <v>1074</v>
       </c>
-    </row>
-    <row r="15" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="P14" s="1">
+        <v>1</v>
+      </c>
+      <c r="Q14" s="1">
+        <v>1</v>
+      </c>
+      <c r="R14" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="15" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A15" s="1" t="s">
         <v>57</v>
       </c>
@@ -20803,8 +20941,17 @@
       <c r="O15" s="1" t="s">
         <v>1074</v>
       </c>
-    </row>
-    <row r="16" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="P15" s="1">
+        <v>1</v>
+      </c>
+      <c r="Q15" s="1">
+        <v>1</v>
+      </c>
+      <c r="R15" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="16" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A16" s="1" t="s">
         <v>61</v>
       </c>
@@ -20850,8 +20997,17 @@
       <c r="O16" s="1" t="s">
         <v>1074</v>
       </c>
-    </row>
-    <row r="17" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="P16" s="1">
+        <v>1</v>
+      </c>
+      <c r="Q16" s="1">
+        <v>1</v>
+      </c>
+      <c r="R16" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="17" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A17" s="1" t="s">
         <v>65</v>
       </c>
@@ -20897,8 +21053,17 @@
       <c r="O17" s="1" t="s">
         <v>1074</v>
       </c>
-    </row>
-    <row r="18" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="P17" s="1">
+        <v>1</v>
+      </c>
+      <c r="Q17" s="1">
+        <v>1</v>
+      </c>
+      <c r="R17" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="18" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A18" s="1" t="s">
         <v>69</v>
       </c>
@@ -20944,8 +21109,17 @@
       <c r="O18" s="1" t="s">
         <v>1074</v>
       </c>
-    </row>
-    <row r="19" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="P18" s="1">
+        <v>1</v>
+      </c>
+      <c r="Q18" s="1">
+        <v>1</v>
+      </c>
+      <c r="R18" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="19" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A19" s="1" t="s">
         <v>71</v>
       </c>
@@ -20991,8 +21165,17 @@
       <c r="O19" s="1" t="s">
         <v>1074</v>
       </c>
-    </row>
-    <row r="20" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="P19" s="1">
+        <v>1</v>
+      </c>
+      <c r="Q19" s="1">
+        <v>1</v>
+      </c>
+      <c r="R19" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="20" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A20" s="1" t="s">
         <v>73</v>
       </c>
@@ -21038,8 +21221,17 @@
       <c r="O20" s="1" t="s">
         <v>1073</v>
       </c>
-    </row>
-    <row r="21" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="P20" s="1">
+        <v>0</v>
+      </c>
+      <c r="Q20" s="1">
+        <v>0</v>
+      </c>
+      <c r="R20" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="21" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A21" s="1" t="s">
         <v>76</v>
       </c>
@@ -21085,8 +21277,17 @@
       <c r="O21" s="1" t="s">
         <v>1073</v>
       </c>
-    </row>
-    <row r="22" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="P21" s="1">
+        <v>1</v>
+      </c>
+      <c r="Q21" s="1">
+        <v>1</v>
+      </c>
+      <c r="R21" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="22" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A22" s="1" t="s">
         <v>79</v>
       </c>
@@ -21132,8 +21333,17 @@
       <c r="O22" s="1" t="s">
         <v>1073</v>
       </c>
-    </row>
-    <row r="23" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="P22" s="1">
+        <v>0</v>
+      </c>
+      <c r="Q22" s="1">
+        <v>0</v>
+      </c>
+      <c r="R22" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="23" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A23" s="1" t="s">
         <v>1003</v>
       </c>
@@ -21179,8 +21389,17 @@
       <c r="O23" s="1" t="s">
         <v>1073</v>
       </c>
-    </row>
-    <row r="24" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="P23" s="1">
+        <v>0</v>
+      </c>
+      <c r="Q23" s="1">
+        <v>0</v>
+      </c>
+      <c r="R23" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="24" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A24" s="1" t="s">
         <v>1004</v>
       </c>
@@ -21226,8 +21445,17 @@
       <c r="O24" s="1" t="s">
         <v>1073</v>
       </c>
-    </row>
-    <row r="25" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="P24" s="1">
+        <v>0</v>
+      </c>
+      <c r="Q24" s="1">
+        <v>0</v>
+      </c>
+      <c r="R24" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="25" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A25" s="1" t="s">
         <v>1005</v>
       </c>
@@ -21273,8 +21501,17 @@
       <c r="O25" s="1" t="s">
         <v>1073</v>
       </c>
-    </row>
-    <row r="26" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="P25" s="1">
+        <v>0</v>
+      </c>
+      <c r="Q25" s="1">
+        <v>0</v>
+      </c>
+      <c r="R25" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="26" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A26" s="1" t="s">
         <v>143</v>
       </c>
@@ -21320,8 +21557,17 @@
       <c r="O26" s="1" t="s">
         <v>1073</v>
       </c>
-    </row>
-    <row r="27" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="P26" s="1">
+        <v>0</v>
+      </c>
+      <c r="Q26" s="1">
+        <v>0</v>
+      </c>
+      <c r="R26" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="27" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A27" s="1" t="s">
         <v>144</v>
       </c>
@@ -21367,8 +21613,17 @@
       <c r="O27" s="1" t="s">
         <v>1073</v>
       </c>
-    </row>
-    <row r="28" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="P27" s="1">
+        <v>0</v>
+      </c>
+      <c r="Q27" s="1">
+        <v>0</v>
+      </c>
+      <c r="R27" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="28" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A28" s="1" t="s">
         <v>145</v>
       </c>
@@ -21414,8 +21669,17 @@
       <c r="O28" s="1" t="s">
         <v>1073</v>
       </c>
-    </row>
-    <row r="29" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="P28" s="1">
+        <v>0</v>
+      </c>
+      <c r="Q28" s="1">
+        <v>0</v>
+      </c>
+      <c r="R28" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="29" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A29" s="1" t="s">
         <v>146</v>
       </c>
@@ -21461,8 +21725,17 @@
       <c r="O29" s="1" t="s">
         <v>1073</v>
       </c>
-    </row>
-    <row r="30" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="P29" s="1">
+        <v>0</v>
+      </c>
+      <c r="Q29" s="1">
+        <v>0</v>
+      </c>
+      <c r="R29" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="30" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A30" s="1" t="s">
         <v>147</v>
       </c>
@@ -21508,8 +21781,17 @@
       <c r="O30" s="1" t="s">
         <v>1073</v>
       </c>
-    </row>
-    <row r="31" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="P30" s="1">
+        <v>0</v>
+      </c>
+      <c r="Q30" s="1">
+        <v>0</v>
+      </c>
+      <c r="R30" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="31" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A31" s="1" t="s">
         <v>148</v>
       </c>
@@ -21549,8 +21831,17 @@
       <c r="O31" s="1" t="s">
         <v>1074</v>
       </c>
-    </row>
-    <row r="32" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="P31" s="1">
+        <v>0</v>
+      </c>
+      <c r="Q31" s="1">
+        <v>0</v>
+      </c>
+      <c r="R31" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="32" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A32" s="1" t="s">
         <v>149</v>
       </c>
@@ -21593,8 +21884,17 @@
       <c r="O32" s="1" t="s">
         <v>1073</v>
       </c>
-    </row>
-    <row r="33" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="P32" s="1">
+        <v>0</v>
+      </c>
+      <c r="Q32" s="1">
+        <v>0</v>
+      </c>
+      <c r="R32" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="33" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A33" s="1" t="s">
         <v>150</v>
       </c>
@@ -21637,8 +21937,17 @@
       <c r="O33" s="1" t="s">
         <v>1074</v>
       </c>
-    </row>
-    <row r="34" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="P33" s="1">
+        <v>0</v>
+      </c>
+      <c r="Q33" s="1">
+        <v>0</v>
+      </c>
+      <c r="R33" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="34" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A34" s="1" t="s">
         <v>151</v>
       </c>
@@ -21681,8 +21990,17 @@
       <c r="O34" s="1" t="s">
         <v>1074</v>
       </c>
-    </row>
-    <row r="35" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="P34" s="1">
+        <v>0</v>
+      </c>
+      <c r="Q34" s="1">
+        <v>0</v>
+      </c>
+      <c r="R34" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="35" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A35" s="1" t="s">
         <v>152</v>
       </c>
@@ -21725,8 +22043,17 @@
       <c r="O35" s="1" t="s">
         <v>1074</v>
       </c>
-    </row>
-    <row r="36" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="P35" s="1">
+        <v>0</v>
+      </c>
+      <c r="Q35" s="1">
+        <v>0</v>
+      </c>
+      <c r="R35" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="36" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A36" s="1" t="s">
         <v>153</v>
       </c>
@@ -21769,8 +22096,17 @@
       <c r="O36" s="1" t="s">
         <v>1074</v>
       </c>
-    </row>
-    <row r="37" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="P36" s="1">
+        <v>1</v>
+      </c>
+      <c r="Q36" s="1">
+        <v>1</v>
+      </c>
+      <c r="R36" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="37" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A37" s="1" t="s">
         <v>154</v>
       </c>
@@ -21813,8 +22149,17 @@
       <c r="O37" s="1" t="s">
         <v>1074</v>
       </c>
-    </row>
-    <row r="38" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="P37" s="1">
+        <v>1</v>
+      </c>
+      <c r="Q37" s="1">
+        <v>1</v>
+      </c>
+      <c r="R37" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="38" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A38" s="1" t="s">
         <v>1006</v>
       </c>
@@ -21857,8 +22202,17 @@
       <c r="O38" s="1" t="s">
         <v>1074</v>
       </c>
-    </row>
-    <row r="39" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="P38" s="1">
+        <v>1</v>
+      </c>
+      <c r="Q38" s="1">
+        <v>1</v>
+      </c>
+      <c r="R38" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="39" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A39" s="1" t="s">
         <v>1007</v>
       </c>
@@ -21901,8 +22255,17 @@
       <c r="O39" s="1" t="s">
         <v>1074</v>
       </c>
-    </row>
-    <row r="40" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="P39" s="1">
+        <v>1</v>
+      </c>
+      <c r="Q39" s="1">
+        <v>1</v>
+      </c>
+      <c r="R39" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="40" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A40" s="1" t="s">
         <v>1008</v>
       </c>
@@ -21945,8 +22308,17 @@
       <c r="O40" s="1" t="s">
         <v>1074</v>
       </c>
-    </row>
-    <row r="41" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="P40" s="1">
+        <v>0</v>
+      </c>
+      <c r="Q40" s="1">
+        <v>0</v>
+      </c>
+      <c r="R40" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="41" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A41" s="1" t="s">
         <v>676</v>
       </c>
@@ -21989,8 +22361,17 @@
       <c r="O41" s="1" t="s">
         <v>1074</v>
       </c>
-    </row>
-    <row r="42" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="P41" s="1">
+        <v>0</v>
+      </c>
+      <c r="Q41" s="1">
+        <v>0</v>
+      </c>
+      <c r="R41" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="42" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A42" s="1" t="s">
         <v>677</v>
       </c>
@@ -22033,8 +22414,17 @@
       <c r="O42" s="1" t="s">
         <v>1074</v>
       </c>
-    </row>
-    <row r="43" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="P42" s="1">
+        <v>0</v>
+      </c>
+      <c r="Q42" s="1">
+        <v>0</v>
+      </c>
+      <c r="R42" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="43" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A43" s="1" t="s">
         <v>678</v>
       </c>
@@ -22077,8 +22467,17 @@
       <c r="O43" s="1" t="s">
         <v>1074</v>
       </c>
-    </row>
-    <row r="44" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="P43" s="1">
+        <v>0</v>
+      </c>
+      <c r="Q43" s="1">
+        <v>0</v>
+      </c>
+      <c r="R43" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="44" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A44" s="1" t="s">
         <v>679</v>
       </c>
@@ -22121,8 +22520,17 @@
       <c r="O44" s="1" t="s">
         <v>1074</v>
       </c>
-    </row>
-    <row r="45" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="P44" s="1">
+        <v>0</v>
+      </c>
+      <c r="Q44" s="1">
+        <v>0</v>
+      </c>
+      <c r="R44" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="45" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A45" s="1" t="s">
         <v>680</v>
       </c>
@@ -22166,8 +22574,17 @@
       <c r="O45" s="1" t="s">
         <v>1074</v>
       </c>
-    </row>
-    <row r="46" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="P45" s="1">
+        <v>0</v>
+      </c>
+      <c r="Q45" s="1">
+        <v>0</v>
+      </c>
+      <c r="R45" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="46" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A46" s="1" t="s">
         <v>681</v>
       </c>
@@ -22210,8 +22627,17 @@
       <c r="O46" s="1" t="s">
         <v>1074</v>
       </c>
-    </row>
-    <row r="47" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="P46" s="1">
+        <v>0</v>
+      </c>
+      <c r="Q46" s="1">
+        <v>0</v>
+      </c>
+      <c r="R46" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="47" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A47" s="1" t="s">
         <v>682</v>
       </c>
@@ -22255,8 +22681,17 @@
       <c r="O47" s="1" t="s">
         <v>1074</v>
       </c>
-    </row>
-    <row r="48" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="P47" s="1">
+        <v>0</v>
+      </c>
+      <c r="Q47" s="1">
+        <v>0</v>
+      </c>
+      <c r="R47" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="48" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A48" s="1" t="s">
         <v>683</v>
       </c>
@@ -22299,8 +22734,17 @@
       <c r="O48" s="1" t="s">
         <v>1074</v>
       </c>
-    </row>
-    <row r="49" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="P48" s="1">
+        <v>0</v>
+      </c>
+      <c r="Q48" s="1">
+        <v>0</v>
+      </c>
+      <c r="R48" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="49" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A49" s="1" t="s">
         <v>684</v>
       </c>
@@ -22343,8 +22787,17 @@
       <c r="O49" s="1" t="s">
         <v>1074</v>
       </c>
-    </row>
-    <row r="50" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="P49" s="1">
+        <v>0</v>
+      </c>
+      <c r="Q49" s="1">
+        <v>0</v>
+      </c>
+      <c r="R49" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="50" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A50" s="1" t="s">
         <v>685</v>
       </c>
@@ -22388,8 +22841,17 @@
       <c r="O50" s="1" t="s">
         <v>1074</v>
       </c>
-    </row>
-    <row r="51" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="P50" s="1">
+        <v>0</v>
+      </c>
+      <c r="Q50" s="1">
+        <v>0</v>
+      </c>
+      <c r="R50" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="51" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A51" s="1" t="s">
         <v>686</v>
       </c>
@@ -22432,8 +22894,17 @@
       <c r="O51" s="1" t="s">
         <v>1074</v>
       </c>
-    </row>
-    <row r="52" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="P51" s="1">
+        <v>0</v>
+      </c>
+      <c r="Q51" s="1">
+        <v>0</v>
+      </c>
+      <c r="R51" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="52" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A52" s="1" t="s">
         <v>687</v>
       </c>
@@ -22476,8 +22947,17 @@
       <c r="O52" s="1" t="s">
         <v>1074</v>
       </c>
-    </row>
-    <row r="53" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="P52" s="1">
+        <v>0</v>
+      </c>
+      <c r="Q52" s="1">
+        <v>0</v>
+      </c>
+      <c r="R52" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="53" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A53" s="1" t="s">
         <v>688</v>
       </c>
@@ -22520,8 +23000,17 @@
       <c r="O53" s="1" t="s">
         <v>1074</v>
       </c>
-    </row>
-    <row r="54" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="P53" s="1">
+        <v>0</v>
+      </c>
+      <c r="Q53" s="1">
+        <v>0</v>
+      </c>
+      <c r="R53" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="54" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A54" s="1" t="s">
         <v>689</v>
       </c>
@@ -22564,8 +23053,17 @@
       <c r="O54" s="1" t="s">
         <v>1074</v>
       </c>
-    </row>
-    <row r="55" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="P54" s="1">
+        <v>0</v>
+      </c>
+      <c r="Q54" s="1">
+        <v>0</v>
+      </c>
+      <c r="R54" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="55" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A55" s="1" t="s">
         <v>690</v>
       </c>
@@ -22608,8 +23106,17 @@
       <c r="O55" s="1" t="s">
         <v>1074</v>
       </c>
-    </row>
-    <row r="56" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="P55" s="1">
+        <v>1</v>
+      </c>
+      <c r="Q55" s="1">
+        <v>1</v>
+      </c>
+      <c r="R55" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="56" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A56" s="1" t="s">
         <v>691</v>
       </c>
@@ -22652,8 +23159,17 @@
       <c r="O56" s="1" t="s">
         <v>1074</v>
       </c>
-    </row>
-    <row r="57" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="P56" s="1">
+        <v>1</v>
+      </c>
+      <c r="Q56" s="1">
+        <v>1</v>
+      </c>
+      <c r="R56" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="57" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A57" s="1" t="s">
         <v>692</v>
       </c>
@@ -22696,8 +23212,17 @@
       <c r="O57" s="1" t="s">
         <v>1074</v>
       </c>
-    </row>
-    <row r="58" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="P57" s="1">
+        <v>1</v>
+      </c>
+      <c r="Q57" s="1">
+        <v>1</v>
+      </c>
+      <c r="R57" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="58" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A58" s="1" t="s">
         <v>693</v>
       </c>
@@ -22740,8 +23265,17 @@
       <c r="O58" s="1" t="s">
         <v>1074</v>
       </c>
-    </row>
-    <row r="59" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="P58" s="1">
+        <v>1</v>
+      </c>
+      <c r="Q58" s="1">
+        <v>1</v>
+      </c>
+      <c r="R58" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="59" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A59" s="1" t="s">
         <v>694</v>
       </c>
@@ -22784,8 +23318,17 @@
       <c r="O59" s="1" t="s">
         <v>1074</v>
       </c>
-    </row>
-    <row r="60" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="P59" s="1">
+        <v>1</v>
+      </c>
+      <c r="Q59" s="1">
+        <v>1</v>
+      </c>
+      <c r="R59" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="60" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A60" s="1" t="s">
         <v>695</v>
       </c>
@@ -22828,8 +23371,17 @@
       <c r="O60" s="1" t="s">
         <v>1074</v>
       </c>
-    </row>
-    <row r="61" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="P60" s="1">
+        <v>1</v>
+      </c>
+      <c r="Q60" s="1">
+        <v>1</v>
+      </c>
+      <c r="R60" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="61" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A61" s="1" t="s">
         <v>696</v>
       </c>
@@ -22872,8 +23424,17 @@
       <c r="O61" s="1" t="s">
         <v>1074</v>
       </c>
-    </row>
-    <row r="62" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="P61" s="1">
+        <v>1</v>
+      </c>
+      <c r="Q61" s="1">
+        <v>1</v>
+      </c>
+      <c r="R61" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="62" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A62" s="1" t="s">
         <v>697</v>
       </c>
@@ -22916,8 +23477,17 @@
       <c r="O62" s="1" t="s">
         <v>1074</v>
       </c>
-    </row>
-    <row r="63" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="P62" s="1">
+        <v>1</v>
+      </c>
+      <c r="Q62" s="1">
+        <v>1</v>
+      </c>
+      <c r="R62" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="63" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A63" s="1" t="s">
         <v>698</v>
       </c>
@@ -22960,8 +23530,17 @@
       <c r="O63" s="1" t="s">
         <v>1074</v>
       </c>
-    </row>
-    <row r="64" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="P63" s="1">
+        <v>1</v>
+      </c>
+      <c r="Q63" s="1">
+        <v>1</v>
+      </c>
+      <c r="R63" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="64" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A64" s="1" t="s">
         <v>699</v>
       </c>
@@ -23004,8 +23583,17 @@
       <c r="O64" s="1" t="s">
         <v>1074</v>
       </c>
-    </row>
-    <row r="65" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="P64" s="1">
+        <v>1</v>
+      </c>
+      <c r="Q64" s="1">
+        <v>1</v>
+      </c>
+      <c r="R64" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="65" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A65" s="1" t="s">
         <v>700</v>
       </c>
@@ -23048,8 +23636,17 @@
       <c r="O65" s="1" t="s">
         <v>1074</v>
       </c>
-    </row>
-    <row r="66" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="P65" s="1">
+        <v>1</v>
+      </c>
+      <c r="Q65" s="1">
+        <v>1</v>
+      </c>
+      <c r="R65" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="66" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A66" s="1" t="s">
         <v>701</v>
       </c>
@@ -23092,8 +23689,17 @@
       <c r="O66" s="1" t="s">
         <v>1074</v>
       </c>
-    </row>
-    <row r="67" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="P66" s="1">
+        <v>1</v>
+      </c>
+      <c r="Q66" s="1">
+        <v>1</v>
+      </c>
+      <c r="R66" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="67" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A67" s="1" t="s">
         <v>702</v>
       </c>
@@ -23136,8 +23742,17 @@
       <c r="O67" s="1" t="s">
         <v>1074</v>
       </c>
-    </row>
-    <row r="68" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="P67" s="1">
+        <v>1</v>
+      </c>
+      <c r="Q67" s="1">
+        <v>1</v>
+      </c>
+      <c r="R67" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="68" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A68" s="1" t="s">
         <v>703</v>
       </c>
@@ -23180,8 +23795,17 @@
       <c r="O68" s="1" t="s">
         <v>1074</v>
       </c>
-    </row>
-    <row r="69" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="P68" s="1">
+        <v>1</v>
+      </c>
+      <c r="Q68" s="1">
+        <v>1</v>
+      </c>
+      <c r="R68" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="69" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A69" s="1" t="s">
         <v>704</v>
       </c>
@@ -23224,8 +23848,17 @@
       <c r="O69" s="1" t="s">
         <v>1074</v>
       </c>
-    </row>
-    <row r="70" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="P69" s="1">
+        <v>1</v>
+      </c>
+      <c r="Q69" s="1">
+        <v>1</v>
+      </c>
+      <c r="R69" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="70" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A70" s="1" t="s">
         <v>705</v>
       </c>
@@ -23268,8 +23901,17 @@
       <c r="O70" s="1" t="s">
         <v>1074</v>
       </c>
-    </row>
-    <row r="71" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="P70" s="1">
+        <v>1</v>
+      </c>
+      <c r="Q70" s="1">
+        <v>1</v>
+      </c>
+      <c r="R70" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="71" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A71" s="1" t="s">
         <v>706</v>
       </c>
@@ -23312,8 +23954,17 @@
       <c r="O71" s="1" t="s">
         <v>1074</v>
       </c>
-    </row>
-    <row r="72" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="P71" s="1">
+        <v>1</v>
+      </c>
+      <c r="Q71" s="1">
+        <v>1</v>
+      </c>
+      <c r="R71" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="72" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A72" s="1" t="s">
         <v>707</v>
       </c>
@@ -23356,8 +24007,17 @@
       <c r="O72" s="1" t="s">
         <v>1074</v>
       </c>
-    </row>
-    <row r="73" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="P72" s="1">
+        <v>1</v>
+      </c>
+      <c r="Q72" s="1">
+        <v>1</v>
+      </c>
+      <c r="R72" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="73" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A73" s="1" t="s">
         <v>708</v>
       </c>
@@ -23400,8 +24060,17 @@
       <c r="O73" s="1" t="s">
         <v>1074</v>
       </c>
-    </row>
-    <row r="74" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="P73" s="1">
+        <v>1</v>
+      </c>
+      <c r="Q73" s="1">
+        <v>1</v>
+      </c>
+      <c r="R73" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="74" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A74" s="1" t="s">
         <v>709</v>
       </c>
@@ -23444,8 +24113,17 @@
       <c r="O74" s="1" t="s">
         <v>1074</v>
       </c>
-    </row>
-    <row r="75" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="P74" s="1">
+        <v>1</v>
+      </c>
+      <c r="Q74" s="1">
+        <v>1</v>
+      </c>
+      <c r="R74" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="75" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A75" s="1" t="s">
         <v>710</v>
       </c>
@@ -23488,8 +24166,17 @@
       <c r="O75" s="1" t="s">
         <v>1074</v>
       </c>
-    </row>
-    <row r="76" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="P75" s="1">
+        <v>1</v>
+      </c>
+      <c r="Q75" s="1">
+        <v>1</v>
+      </c>
+      <c r="R75" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="76" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A76" s="1" t="s">
         <v>711</v>
       </c>
@@ -23532,8 +24219,17 @@
       <c r="O76" s="1" t="s">
         <v>1074</v>
       </c>
-    </row>
-    <row r="77" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="P76" s="1">
+        <v>1</v>
+      </c>
+      <c r="Q76" s="1">
+        <v>1</v>
+      </c>
+      <c r="R76" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="77" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A77" s="1" t="s">
         <v>712</v>
       </c>
@@ -23576,8 +24272,17 @@
       <c r="O77" s="1" t="s">
         <v>1074</v>
       </c>
-    </row>
-    <row r="78" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="P77" s="1">
+        <v>0</v>
+      </c>
+      <c r="Q77" s="1">
+        <v>0</v>
+      </c>
+      <c r="R77" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="78" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A78" s="1" t="s">
         <v>713</v>
       </c>
@@ -23620,8 +24325,17 @@
       <c r="O78" s="1" t="s">
         <v>1074</v>
       </c>
-    </row>
-    <row r="79" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="P78" s="1">
+        <v>0</v>
+      </c>
+      <c r="Q78" s="1">
+        <v>0</v>
+      </c>
+      <c r="R78" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="79" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A79" s="1" t="s">
         <v>714</v>
       </c>
@@ -23664,8 +24378,17 @@
       <c r="O79" s="1" t="s">
         <v>1074</v>
       </c>
-    </row>
-    <row r="80" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="P79" s="1">
+        <v>0</v>
+      </c>
+      <c r="Q79" s="1">
+        <v>0</v>
+      </c>
+      <c r="R79" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="80" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A80" s="1" t="s">
         <v>715</v>
       </c>
@@ -23708,8 +24431,17 @@
       <c r="O80" s="1" t="s">
         <v>1074</v>
       </c>
-    </row>
-    <row r="81" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="P80" s="1">
+        <v>0</v>
+      </c>
+      <c r="Q80" s="1">
+        <v>0</v>
+      </c>
+      <c r="R80" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="81" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A81" s="1" t="s">
         <v>716</v>
       </c>
@@ -23752,8 +24484,17 @@
       <c r="O81" s="1" t="s">
         <v>1074</v>
       </c>
-    </row>
-    <row r="82" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="P81" s="1">
+        <v>0</v>
+      </c>
+      <c r="Q81" s="1">
+        <v>0</v>
+      </c>
+      <c r="R81" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="82" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A82" s="1" t="s">
         <v>717</v>
       </c>
@@ -23796,8 +24537,17 @@
       <c r="O82" s="1" t="s">
         <v>1074</v>
       </c>
-    </row>
-    <row r="83" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="P82" s="1">
+        <v>0</v>
+      </c>
+      <c r="Q82" s="1">
+        <v>0</v>
+      </c>
+      <c r="R82" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="83" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A83" s="1" t="s">
         <v>718</v>
       </c>
@@ -23840,8 +24590,17 @@
       <c r="O83" s="1" t="s">
         <v>1074</v>
       </c>
-    </row>
-    <row r="84" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="P83" s="1">
+        <v>0</v>
+      </c>
+      <c r="Q83" s="1">
+        <v>0</v>
+      </c>
+      <c r="R83" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="84" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A84" s="1" t="s">
         <v>719</v>
       </c>
@@ -23884,8 +24643,17 @@
       <c r="O84" s="1" t="s">
         <v>1074</v>
       </c>
-    </row>
-    <row r="85" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="P84" s="1">
+        <v>1</v>
+      </c>
+      <c r="Q84" s="1">
+        <v>1</v>
+      </c>
+      <c r="R84" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="85" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A85" s="1" t="s">
         <v>720</v>
       </c>
@@ -23928,8 +24696,17 @@
       <c r="O85" s="1" t="s">
         <v>1074</v>
       </c>
-    </row>
-    <row r="86" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="P85" s="1">
+        <v>1</v>
+      </c>
+      <c r="Q85" s="1">
+        <v>1</v>
+      </c>
+      <c r="R85" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="86" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A86" s="1" t="s">
         <v>721</v>
       </c>
@@ -23972,8 +24749,17 @@
       <c r="O86" s="1" t="s">
         <v>1074</v>
       </c>
-    </row>
-    <row r="87" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="P86" s="1">
+        <v>1</v>
+      </c>
+      <c r="Q86" s="1">
+        <v>1</v>
+      </c>
+      <c r="R86" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="87" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A87" s="1" t="s">
         <v>722</v>
       </c>
@@ -24016,8 +24802,17 @@
       <c r="O87" s="1" t="s">
         <v>1074</v>
       </c>
-    </row>
-    <row r="88" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="P87" s="1">
+        <v>1</v>
+      </c>
+      <c r="Q87" s="1">
+        <v>1</v>
+      </c>
+      <c r="R87" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="88" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A88" s="1" t="s">
         <v>723</v>
       </c>
@@ -24060,8 +24855,17 @@
       <c r="O88" s="1" t="s">
         <v>1074</v>
       </c>
-    </row>
-    <row r="89" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="P88" s="1">
+        <v>1</v>
+      </c>
+      <c r="Q88" s="1">
+        <v>1</v>
+      </c>
+      <c r="R88" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="89" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A89" s="1" t="s">
         <v>724</v>
       </c>
@@ -24104,8 +24908,17 @@
       <c r="O89" s="1" t="s">
         <v>1074</v>
       </c>
-    </row>
-    <row r="90" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="P89" s="1">
+        <v>0</v>
+      </c>
+      <c r="Q89" s="1">
+        <v>0</v>
+      </c>
+      <c r="R89" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="90" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A90" s="1" t="s">
         <v>725</v>
       </c>
@@ -24148,8 +24961,17 @@
       <c r="O90" s="1" t="s">
         <v>1074</v>
       </c>
-    </row>
-    <row r="91" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="P90" s="1">
+        <v>1</v>
+      </c>
+      <c r="Q90" s="1">
+        <v>1</v>
+      </c>
+      <c r="R90" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="91" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A91" s="1" t="s">
         <v>726</v>
       </c>
@@ -24192,8 +25014,17 @@
       <c r="O91" s="1" t="s">
         <v>1074</v>
       </c>
-    </row>
-    <row r="92" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="P91" s="1">
+        <v>1</v>
+      </c>
+      <c r="Q91" s="1">
+        <v>1</v>
+      </c>
+      <c r="R91" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="92" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A92" s="1" t="s">
         <v>727</v>
       </c>
@@ -24236,8 +25067,17 @@
       <c r="O92" s="1" t="s">
         <v>1074</v>
       </c>
-    </row>
-    <row r="93" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="P92" s="1">
+        <v>1</v>
+      </c>
+      <c r="Q92" s="1">
+        <v>1</v>
+      </c>
+      <c r="R92" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="93" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A93" s="1" t="s">
         <v>728</v>
       </c>
@@ -24280,8 +25120,17 @@
       <c r="O93" s="1" t="s">
         <v>1074</v>
       </c>
-    </row>
-    <row r="94" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="P93" s="1">
+        <v>1</v>
+      </c>
+      <c r="Q93" s="1">
+        <v>1</v>
+      </c>
+      <c r="R93" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="94" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A94" s="1" t="s">
         <v>729</v>
       </c>
@@ -24324,8 +25173,17 @@
       <c r="O94" s="1" t="s">
         <v>1074</v>
       </c>
-    </row>
-    <row r="95" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="P94" s="1">
+        <v>1</v>
+      </c>
+      <c r="Q94" s="1">
+        <v>1</v>
+      </c>
+      <c r="R94" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="95" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A95" s="1" t="s">
         <v>730</v>
       </c>
@@ -24368,8 +25226,17 @@
       <c r="O95" s="1" t="s">
         <v>1074</v>
       </c>
-    </row>
-    <row r="96" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="P95" s="1">
+        <v>1</v>
+      </c>
+      <c r="Q95" s="1">
+        <v>1</v>
+      </c>
+      <c r="R95" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="96" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A96" s="1" t="s">
         <v>731</v>
       </c>
@@ -24412,8 +25279,17 @@
       <c r="O96" s="1" t="s">
         <v>1074</v>
       </c>
-    </row>
-    <row r="97" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="P96" s="1">
+        <v>1</v>
+      </c>
+      <c r="Q96" s="1">
+        <v>1</v>
+      </c>
+      <c r="R96" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="97" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A97" s="1" t="s">
         <v>732</v>
       </c>
@@ -24456,8 +25332,17 @@
       <c r="O97" s="1" t="s">
         <v>1074</v>
       </c>
-    </row>
-    <row r="98" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="P97" s="1">
+        <v>1</v>
+      </c>
+      <c r="Q97" s="1">
+        <v>1</v>
+      </c>
+      <c r="R97" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="98" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A98" s="1" t="s">
         <v>733</v>
       </c>
@@ -24500,8 +25385,17 @@
       <c r="O98" s="1" t="s">
         <v>1074</v>
       </c>
-    </row>
-    <row r="99" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="P98" s="1">
+        <v>1</v>
+      </c>
+      <c r="Q98" s="1">
+        <v>1</v>
+      </c>
+      <c r="R98" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="99" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A99" s="1" t="s">
         <v>734</v>
       </c>
@@ -24544,8 +25438,17 @@
       <c r="O99" s="1" t="s">
         <v>1074</v>
       </c>
-    </row>
-    <row r="100" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="P99" s="1">
+        <v>1</v>
+      </c>
+      <c r="Q99" s="1">
+        <v>1</v>
+      </c>
+      <c r="R99" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="100" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A100" s="1" t="s">
         <v>735</v>
       </c>
@@ -24588,8 +25491,17 @@
       <c r="O100" s="1" t="s">
         <v>1074</v>
       </c>
-    </row>
-    <row r="101" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="P100" s="1">
+        <v>1</v>
+      </c>
+      <c r="Q100" s="1">
+        <v>1</v>
+      </c>
+      <c r="R100" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="101" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A101" s="1" t="s">
         <v>736</v>
       </c>
@@ -24632,8 +25544,17 @@
       <c r="O101" s="1" t="s">
         <v>1074</v>
       </c>
-    </row>
-    <row r="102" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="P101" s="1">
+        <v>1</v>
+      </c>
+      <c r="Q101" s="1">
+        <v>1</v>
+      </c>
+      <c r="R101" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="102" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A102" s="1" t="s">
         <v>737</v>
       </c>
@@ -24676,8 +25597,17 @@
       <c r="O102" s="1" t="s">
         <v>1074</v>
       </c>
-    </row>
-    <row r="103" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="P102" s="1">
+        <v>1</v>
+      </c>
+      <c r="Q102" s="1">
+        <v>1</v>
+      </c>
+      <c r="R102" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="103" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A103" s="1" t="s">
         <v>738</v>
       </c>
@@ -24720,8 +25650,17 @@
       <c r="O103" s="1" t="s">
         <v>1074</v>
       </c>
-    </row>
-    <row r="104" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="P103" s="1">
+        <v>1</v>
+      </c>
+      <c r="Q103" s="1">
+        <v>1</v>
+      </c>
+      <c r="R103" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="104" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A104" s="1" t="s">
         <v>739</v>
       </c>
@@ -24764,8 +25703,17 @@
       <c r="O104" s="1" t="s">
         <v>1074</v>
       </c>
-    </row>
-    <row r="105" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="P104" s="1">
+        <v>1</v>
+      </c>
+      <c r="Q104" s="1">
+        <v>1</v>
+      </c>
+      <c r="R104" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="105" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A105" s="1" t="s">
         <v>740</v>
       </c>
@@ -24808,8 +25756,17 @@
       <c r="O105" s="1" t="s">
         <v>1074</v>
       </c>
-    </row>
-    <row r="106" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="P105" s="1">
+        <v>1</v>
+      </c>
+      <c r="Q105" s="1">
+        <v>1</v>
+      </c>
+      <c r="R105" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="106" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A106" s="1" t="s">
         <v>741</v>
       </c>
@@ -24852,8 +25809,17 @@
       <c r="O106" s="1" t="s">
         <v>1074</v>
       </c>
-    </row>
-    <row r="107" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="P106" s="1">
+        <v>1</v>
+      </c>
+      <c r="Q106" s="1">
+        <v>1</v>
+      </c>
+      <c r="R106" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="107" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A107" s="1" t="s">
         <v>742</v>
       </c>
@@ -24896,8 +25862,17 @@
       <c r="O107" s="1" t="s">
         <v>1074</v>
       </c>
-    </row>
-    <row r="108" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="P107" s="1">
+        <v>1</v>
+      </c>
+      <c r="Q107" s="1">
+        <v>1</v>
+      </c>
+      <c r="R107" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="108" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A108" s="1" t="s">
         <v>743</v>
       </c>
@@ -24940,8 +25915,17 @@
       <c r="O108" s="1" t="s">
         <v>1074</v>
       </c>
-    </row>
-    <row r="109" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="P108" s="1">
+        <v>1</v>
+      </c>
+      <c r="Q108" s="1">
+        <v>1</v>
+      </c>
+      <c r="R108" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="109" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A109" s="1" t="s">
         <v>744</v>
       </c>
@@ -24984,8 +25968,17 @@
       <c r="O109" s="1" t="s">
         <v>1074</v>
       </c>
-    </row>
-    <row r="110" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="P109" s="1">
+        <v>1</v>
+      </c>
+      <c r="Q109" s="1">
+        <v>1</v>
+      </c>
+      <c r="R109" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="110" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A110" s="1" t="s">
         <v>745</v>
       </c>
@@ -25028,8 +26021,17 @@
       <c r="O110" s="1" t="s">
         <v>1074</v>
       </c>
-    </row>
-    <row r="111" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="P110" s="1">
+        <v>1</v>
+      </c>
+      <c r="Q110" s="1">
+        <v>1</v>
+      </c>
+      <c r="R110" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="111" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A111" s="1" t="s">
         <v>746</v>
       </c>
@@ -25072,8 +26074,17 @@
       <c r="O111" s="1" t="s">
         <v>1074</v>
       </c>
-    </row>
-    <row r="112" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="P111" s="1">
+        <v>1</v>
+      </c>
+      <c r="Q111" s="1">
+        <v>1</v>
+      </c>
+      <c r="R111" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="112" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A112" s="1" t="s">
         <v>747</v>
       </c>
@@ -25116,8 +26127,17 @@
       <c r="O112" s="1" t="s">
         <v>1074</v>
       </c>
-    </row>
-    <row r="113" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="P112" s="1">
+        <v>1</v>
+      </c>
+      <c r="Q112" s="1">
+        <v>1</v>
+      </c>
+      <c r="R112" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="113" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A113" s="1" t="s">
         <v>748</v>
       </c>
@@ -25160,8 +26180,17 @@
       <c r="O113" s="1" t="s">
         <v>1074</v>
       </c>
-    </row>
-    <row r="114" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="P113" s="1">
+        <v>1</v>
+      </c>
+      <c r="Q113" s="1">
+        <v>1</v>
+      </c>
+      <c r="R113" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="114" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A114" s="1" t="s">
         <v>749</v>
       </c>
@@ -25204,8 +26233,17 @@
       <c r="O114" s="1" t="s">
         <v>1074</v>
       </c>
-    </row>
-    <row r="115" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="P114" s="1">
+        <v>1</v>
+      </c>
+      <c r="Q114" s="1">
+        <v>1</v>
+      </c>
+      <c r="R114" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="115" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A115" s="1" t="s">
         <v>750</v>
       </c>
@@ -25248,8 +26286,17 @@
       <c r="O115" s="1" t="s">
         <v>1074</v>
       </c>
-    </row>
-    <row r="116" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="P115" s="1">
+        <v>1</v>
+      </c>
+      <c r="Q115" s="1">
+        <v>1</v>
+      </c>
+      <c r="R115" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="116" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A116" s="1" t="s">
         <v>751</v>
       </c>
@@ -25292,8 +26339,17 @@
       <c r="O116" s="1" t="s">
         <v>1074</v>
       </c>
-    </row>
-    <row r="117" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="P116" s="1">
+        <v>1</v>
+      </c>
+      <c r="Q116" s="1">
+        <v>1</v>
+      </c>
+      <c r="R116" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="117" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A117" s="1" t="s">
         <v>752</v>
       </c>
@@ -25336,8 +26392,17 @@
       <c r="O117" s="1" t="s">
         <v>1074</v>
       </c>
-    </row>
-    <row r="118" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="P117" s="1">
+        <v>0</v>
+      </c>
+      <c r="Q117" s="1">
+        <v>0</v>
+      </c>
+      <c r="R117" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="118" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A118" s="1" t="s">
         <v>753</v>
       </c>
@@ -25380,8 +26445,17 @@
       <c r="O118" s="1" t="s">
         <v>1074</v>
       </c>
-    </row>
-    <row r="119" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="P118" s="1">
+        <v>0</v>
+      </c>
+      <c r="Q118" s="1">
+        <v>0</v>
+      </c>
+      <c r="R118" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="119" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A119" s="1" t="s">
         <v>754</v>
       </c>
@@ -25424,8 +26498,17 @@
       <c r="O119" s="1" t="s">
         <v>1074</v>
       </c>
-    </row>
-    <row r="120" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="P119" s="1">
+        <v>0</v>
+      </c>
+      <c r="Q119" s="1">
+        <v>0</v>
+      </c>
+      <c r="R119" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="120" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A120" s="1" t="s">
         <v>755</v>
       </c>
@@ -25468,8 +26551,17 @@
       <c r="O120" s="1" t="s">
         <v>1074</v>
       </c>
-    </row>
-    <row r="121" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="P120" s="1">
+        <v>0</v>
+      </c>
+      <c r="Q120" s="1">
+        <v>0</v>
+      </c>
+      <c r="R120" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="121" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A121" s="1" t="s">
         <v>756</v>
       </c>
@@ -25512,8 +26604,17 @@
       <c r="O121" s="1" t="s">
         <v>1074</v>
       </c>
-    </row>
-    <row r="122" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="P121" s="1">
+        <v>0</v>
+      </c>
+      <c r="Q121" s="1">
+        <v>0</v>
+      </c>
+      <c r="R121" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="122" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A122" s="1" t="s">
         <v>757</v>
       </c>
@@ -25556,8 +26657,17 @@
       <c r="O122" s="1" t="s">
         <v>1074</v>
       </c>
-    </row>
-    <row r="123" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="P122" s="1">
+        <v>0</v>
+      </c>
+      <c r="Q122" s="1">
+        <v>0</v>
+      </c>
+      <c r="R122" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="123" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A123" s="1" t="s">
         <v>758</v>
       </c>
@@ -25600,8 +26710,17 @@
       <c r="O123" s="1" t="s">
         <v>1074</v>
       </c>
-    </row>
-    <row r="124" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="P123" s="1">
+        <v>0</v>
+      </c>
+      <c r="Q123" s="1">
+        <v>0</v>
+      </c>
+      <c r="R123" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="124" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A124" s="1" t="s">
         <v>759</v>
       </c>
@@ -25644,8 +26763,17 @@
       <c r="O124" s="1" t="s">
         <v>1074</v>
       </c>
-    </row>
-    <row r="125" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="P124" s="1">
+        <v>0</v>
+      </c>
+      <c r="Q124" s="1">
+        <v>0</v>
+      </c>
+      <c r="R124" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="125" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A125" s="1" t="s">
         <v>760</v>
       </c>
@@ -25688,8 +26816,17 @@
       <c r="O125" s="1" t="s">
         <v>1074</v>
       </c>
-    </row>
-    <row r="126" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="P125" s="1">
+        <v>0</v>
+      </c>
+      <c r="Q125" s="1">
+        <v>0</v>
+      </c>
+      <c r="R125" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="126" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A126" s="1" t="s">
         <v>761</v>
       </c>
@@ -25732,8 +26869,17 @@
       <c r="O126" s="1" t="s">
         <v>1074</v>
       </c>
-    </row>
-    <row r="127" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="P126" s="1">
+        <v>0</v>
+      </c>
+      <c r="Q126" s="1">
+        <v>0</v>
+      </c>
+      <c r="R126" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="127" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A127" s="1" t="s">
         <v>762</v>
       </c>
@@ -25776,8 +26922,17 @@
       <c r="O127" s="1" t="s">
         <v>1074</v>
       </c>
-    </row>
-    <row r="128" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="P127" s="1">
+        <v>0</v>
+      </c>
+      <c r="Q127" s="1">
+        <v>0</v>
+      </c>
+      <c r="R127" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="128" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A128" s="1" t="s">
         <v>763</v>
       </c>
@@ -25820,8 +26975,17 @@
       <c r="O128" s="1" t="s">
         <v>1074</v>
       </c>
-    </row>
-    <row r="129" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="P128" s="1">
+        <v>0</v>
+      </c>
+      <c r="Q128" s="1">
+        <v>0</v>
+      </c>
+      <c r="R128" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="129" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A129" s="1" t="s">
         <v>764</v>
       </c>
@@ -25864,8 +27028,17 @@
       <c r="O129" s="1" t="s">
         <v>1074</v>
       </c>
-    </row>
-    <row r="130" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="P129" s="1">
+        <v>0</v>
+      </c>
+      <c r="Q129" s="1">
+        <v>0</v>
+      </c>
+      <c r="R129" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="130" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A130" s="1" t="s">
         <v>765</v>
       </c>
@@ -25908,8 +27081,17 @@
       <c r="O130" s="1" t="s">
         <v>1074</v>
       </c>
-    </row>
-    <row r="131" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="P130" s="1">
+        <v>0</v>
+      </c>
+      <c r="Q130" s="1">
+        <v>0</v>
+      </c>
+      <c r="R130" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="131" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A131" s="1" t="s">
         <v>766</v>
       </c>
@@ -25952,8 +27134,17 @@
       <c r="O131" s="1" t="s">
         <v>1074</v>
       </c>
-    </row>
-    <row r="132" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="P131" s="1">
+        <v>0</v>
+      </c>
+      <c r="Q131" s="1">
+        <v>0</v>
+      </c>
+      <c r="R131" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="132" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A132" s="1" t="s">
         <v>767</v>
       </c>
@@ -25996,8 +27187,17 @@
       <c r="O132" s="1" t="s">
         <v>1074</v>
       </c>
-    </row>
-    <row r="133" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="P132" s="1">
+        <v>0</v>
+      </c>
+      <c r="Q132" s="1">
+        <v>0</v>
+      </c>
+      <c r="R132" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="133" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A133" s="1" t="s">
         <v>768</v>
       </c>
@@ -26040,8 +27240,17 @@
       <c r="O133" s="1" t="s">
         <v>1074</v>
       </c>
-    </row>
-    <row r="134" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="P133" s="1">
+        <v>0</v>
+      </c>
+      <c r="Q133" s="1">
+        <v>0</v>
+      </c>
+      <c r="R133" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="134" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A134" s="1" t="s">
         <v>769</v>
       </c>
@@ -26084,8 +27293,17 @@
       <c r="O134" s="1" t="s">
         <v>1074</v>
       </c>
-    </row>
-    <row r="135" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="P134" s="1">
+        <v>0</v>
+      </c>
+      <c r="Q134" s="1">
+        <v>0</v>
+      </c>
+      <c r="R134" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="135" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A135" s="1" t="s">
         <v>770</v>
       </c>
@@ -26128,8 +27346,17 @@
       <c r="O135" s="1" t="s">
         <v>1074</v>
       </c>
-    </row>
-    <row r="136" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="P135" s="1">
+        <v>0</v>
+      </c>
+      <c r="Q135" s="1">
+        <v>0</v>
+      </c>
+      <c r="R135" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="136" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A136" s="1" t="s">
         <v>771</v>
       </c>
@@ -26172,8 +27399,17 @@
       <c r="O136" s="1" t="s">
         <v>1074</v>
       </c>
-    </row>
-    <row r="137" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="P136" s="1">
+        <v>0</v>
+      </c>
+      <c r="Q136" s="1">
+        <v>0</v>
+      </c>
+      <c r="R136" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="137" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A137" s="1" t="s">
         <v>772</v>
       </c>
@@ -26216,8 +27452,17 @@
       <c r="O137" s="1" t="s">
         <v>1074</v>
       </c>
-    </row>
-    <row r="138" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="P137" s="1">
+        <v>0</v>
+      </c>
+      <c r="Q137" s="1">
+        <v>0</v>
+      </c>
+      <c r="R137" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="138" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A138" s="1" t="s">
         <v>773</v>
       </c>
@@ -26260,8 +27505,17 @@
       <c r="O138" s="1" t="s">
         <v>1074</v>
       </c>
-    </row>
-    <row r="139" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="P138" s="1">
+        <v>0</v>
+      </c>
+      <c r="Q138" s="1">
+        <v>0</v>
+      </c>
+      <c r="R138" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="139" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A139" s="1" t="s">
         <v>774</v>
       </c>
@@ -26304,8 +27558,17 @@
       <c r="O139" s="1" t="s">
         <v>1074</v>
       </c>
-    </row>
-    <row r="140" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="P139" s="1">
+        <v>0</v>
+      </c>
+      <c r="Q139" s="1">
+        <v>0</v>
+      </c>
+      <c r="R139" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="140" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A140" s="1" t="s">
         <v>775</v>
       </c>
@@ -26348,8 +27611,17 @@
       <c r="O140" s="1" t="s">
         <v>1074</v>
       </c>
-    </row>
-    <row r="141" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="P140" s="1">
+        <v>0</v>
+      </c>
+      <c r="Q140" s="1">
+        <v>0</v>
+      </c>
+      <c r="R140" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="141" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A141" s="1" t="s">
         <v>776</v>
       </c>
@@ -26392,8 +27664,17 @@
       <c r="O141" s="1" t="s">
         <v>1074</v>
       </c>
-    </row>
-    <row r="142" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="P141" s="1">
+        <v>0</v>
+      </c>
+      <c r="Q141" s="1">
+        <v>0</v>
+      </c>
+      <c r="R141" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="142" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A142" s="1" t="s">
         <v>777</v>
       </c>
@@ -26436,8 +27717,17 @@
       <c r="O142" s="1" t="s">
         <v>1074</v>
       </c>
-    </row>
-    <row r="143" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="P142" s="1">
+        <v>0</v>
+      </c>
+      <c r="Q142" s="1">
+        <v>0</v>
+      </c>
+      <c r="R142" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="143" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A143" s="1" t="s">
         <v>778</v>
       </c>
@@ -26480,8 +27770,17 @@
       <c r="O143" s="1" t="s">
         <v>1074</v>
       </c>
-    </row>
-    <row r="144" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="P143" s="1">
+        <v>0</v>
+      </c>
+      <c r="Q143" s="1">
+        <v>0</v>
+      </c>
+      <c r="R143" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="144" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A144" s="1" t="s">
         <v>779</v>
       </c>
@@ -26524,8 +27823,17 @@
       <c r="O144" s="1" t="s">
         <v>1074</v>
       </c>
-    </row>
-    <row r="145" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="P144" s="1">
+        <v>0</v>
+      </c>
+      <c r="Q144" s="1">
+        <v>0</v>
+      </c>
+      <c r="R144" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="145" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A145" s="1" t="s">
         <v>780</v>
       </c>
@@ -26568,8 +27876,17 @@
       <c r="O145" s="1" t="s">
         <v>1074</v>
       </c>
-    </row>
-    <row r="146" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="P145" s="1">
+        <v>0</v>
+      </c>
+      <c r="Q145" s="1">
+        <v>0</v>
+      </c>
+      <c r="R145" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="146" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A146" s="1" t="s">
         <v>781</v>
       </c>
@@ -26612,8 +27929,17 @@
       <c r="O146" s="1" t="s">
         <v>1074</v>
       </c>
-    </row>
-    <row r="147" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="P146" s="1">
+        <v>0</v>
+      </c>
+      <c r="Q146" s="1">
+        <v>0</v>
+      </c>
+      <c r="R146" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="147" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A147" s="1" t="s">
         <v>782</v>
       </c>
@@ -26656,8 +27982,17 @@
       <c r="O147" s="1" t="s">
         <v>1074</v>
       </c>
-    </row>
-    <row r="148" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="P147" s="1">
+        <v>0</v>
+      </c>
+      <c r="Q147" s="1">
+        <v>0</v>
+      </c>
+      <c r="R147" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="148" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A148" s="1" t="s">
         <v>783</v>
       </c>
@@ -26700,8 +28035,17 @@
       <c r="O148" s="1" t="s">
         <v>1074</v>
       </c>
-    </row>
-    <row r="149" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="P148" s="1">
+        <v>0</v>
+      </c>
+      <c r="Q148" s="1">
+        <v>0</v>
+      </c>
+      <c r="R148" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="149" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A149" s="1" t="s">
         <v>784</v>
       </c>
@@ -26744,8 +28088,17 @@
       <c r="O149" s="1" t="s">
         <v>1074</v>
       </c>
-    </row>
-    <row r="150" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="P149" s="1">
+        <v>0</v>
+      </c>
+      <c r="Q149" s="1">
+        <v>0</v>
+      </c>
+      <c r="R149" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="150" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A150" s="1" t="s">
         <v>785</v>
       </c>
@@ -26788,8 +28141,17 @@
       <c r="O150" s="1" t="s">
         <v>1074</v>
       </c>
-    </row>
-    <row r="151" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="P150" s="1">
+        <v>0</v>
+      </c>
+      <c r="Q150" s="1">
+        <v>0</v>
+      </c>
+      <c r="R150" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="151" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A151" s="1" t="s">
         <v>786</v>
       </c>
@@ -26832,8 +28194,17 @@
       <c r="O151" s="1" t="s">
         <v>1074</v>
       </c>
-    </row>
-    <row r="152" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="P151" s="1">
+        <v>0</v>
+      </c>
+      <c r="Q151" s="1">
+        <v>0</v>
+      </c>
+      <c r="R151" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="152" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A152" s="1" t="s">
         <v>787</v>
       </c>
@@ -26876,8 +28247,17 @@
       <c r="O152" s="1" t="s">
         <v>1074</v>
       </c>
-    </row>
-    <row r="153" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="P152" s="1">
+        <v>0</v>
+      </c>
+      <c r="Q152" s="1">
+        <v>0</v>
+      </c>
+      <c r="R152" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="153" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A153" s="1" t="s">
         <v>788</v>
       </c>
@@ -26920,8 +28300,17 @@
       <c r="O153" s="1" t="s">
         <v>1074</v>
       </c>
-    </row>
-    <row r="154" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="P153" s="1">
+        <v>0</v>
+      </c>
+      <c r="Q153" s="1">
+        <v>0</v>
+      </c>
+      <c r="R153" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="154" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A154" s="1" t="s">
         <v>789</v>
       </c>
@@ -26964,8 +28353,17 @@
       <c r="O154" s="1" t="s">
         <v>1074</v>
       </c>
-    </row>
-    <row r="155" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="P154" s="1">
+        <v>0</v>
+      </c>
+      <c r="Q154" s="1">
+        <v>0</v>
+      </c>
+      <c r="R154" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="155" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A155" s="1" t="s">
         <v>790</v>
       </c>
@@ -27008,8 +28406,17 @@
       <c r="O155" s="1" t="s">
         <v>1074</v>
       </c>
-    </row>
-    <row r="156" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="P155" s="1">
+        <v>0</v>
+      </c>
+      <c r="Q155" s="1">
+        <v>0</v>
+      </c>
+      <c r="R155" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="156" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A156" s="1" t="s">
         <v>791</v>
       </c>
@@ -27052,8 +28459,17 @@
       <c r="O156" s="1" t="s">
         <v>1074</v>
       </c>
-    </row>
-    <row r="157" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="P156" s="1">
+        <v>0</v>
+      </c>
+      <c r="Q156" s="1">
+        <v>0</v>
+      </c>
+      <c r="R156" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="157" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A157" s="1" t="s">
         <v>792</v>
       </c>
@@ -27096,8 +28512,17 @@
       <c r="O157" s="1" t="s">
         <v>1074</v>
       </c>
-    </row>
-    <row r="158" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="P157" s="1">
+        <v>0</v>
+      </c>
+      <c r="Q157" s="1">
+        <v>0</v>
+      </c>
+      <c r="R157" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="158" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A158" s="1" t="s">
         <v>793</v>
       </c>
@@ -27140,8 +28565,17 @@
       <c r="O158" s="1" t="s">
         <v>1074</v>
       </c>
-    </row>
-    <row r="159" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="P158" s="1">
+        <v>0</v>
+      </c>
+      <c r="Q158" s="1">
+        <v>0</v>
+      </c>
+      <c r="R158" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="159" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A159" s="1" t="s">
         <v>794</v>
       </c>
@@ -27184,8 +28618,17 @@
       <c r="O159" s="1" t="s">
         <v>1074</v>
       </c>
-    </row>
-    <row r="160" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="P159" s="1">
+        <v>0</v>
+      </c>
+      <c r="Q159" s="1">
+        <v>0</v>
+      </c>
+      <c r="R159" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="160" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A160" s="1" t="s">
         <v>795</v>
       </c>
@@ -27228,8 +28671,17 @@
       <c r="O160" s="1" t="s">
         <v>1074</v>
       </c>
-    </row>
-    <row r="161" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="P160" s="1">
+        <v>0</v>
+      </c>
+      <c r="Q160" s="1">
+        <v>0</v>
+      </c>
+      <c r="R160" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="161" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A161" s="1" t="s">
         <v>796</v>
       </c>
@@ -27272,8 +28724,17 @@
       <c r="O161" s="1" t="s">
         <v>1074</v>
       </c>
-    </row>
-    <row r="162" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="P161" s="1">
+        <v>0</v>
+      </c>
+      <c r="Q161" s="1">
+        <v>0</v>
+      </c>
+      <c r="R161" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="162" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A162" s="1" t="s">
         <v>797</v>
       </c>
@@ -27316,8 +28777,17 @@
       <c r="O162" s="1" t="s">
         <v>1074</v>
       </c>
-    </row>
-    <row r="163" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="P162" s="1">
+        <v>0</v>
+      </c>
+      <c r="Q162" s="1">
+        <v>0</v>
+      </c>
+      <c r="R162" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="163" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A163" s="1" t="s">
         <v>798</v>
       </c>
@@ -27360,8 +28830,17 @@
       <c r="O163" s="1" t="s">
         <v>1074</v>
       </c>
-    </row>
-    <row r="164" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="P163" s="1">
+        <v>0</v>
+      </c>
+      <c r="Q163" s="1">
+        <v>0</v>
+      </c>
+      <c r="R163" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="164" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A164" s="1" t="s">
         <v>799</v>
       </c>
@@ -27404,8 +28883,17 @@
       <c r="O164" s="1" t="s">
         <v>1074</v>
       </c>
-    </row>
-    <row r="165" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="P164" s="1">
+        <v>0</v>
+      </c>
+      <c r="Q164" s="1">
+        <v>0</v>
+      </c>
+      <c r="R164" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="165" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A165" s="1" t="s">
         <v>800</v>
       </c>
@@ -27448,8 +28936,17 @@
       <c r="O165" s="1" t="s">
         <v>1074</v>
       </c>
-    </row>
-    <row r="166" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="P165" s="1">
+        <v>0</v>
+      </c>
+      <c r="Q165" s="1">
+        <v>0</v>
+      </c>
+      <c r="R165" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="166" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A166" s="1" t="s">
         <v>801</v>
       </c>
@@ -27492,8 +28989,17 @@
       <c r="O166" s="1" t="s">
         <v>1074</v>
       </c>
-    </row>
-    <row r="167" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="P166" s="1">
+        <v>0</v>
+      </c>
+      <c r="Q166" s="1">
+        <v>0</v>
+      </c>
+      <c r="R166" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="167" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A167" s="1" t="s">
         <v>802</v>
       </c>
@@ -27536,8 +29042,17 @@
       <c r="O167" s="1" t="s">
         <v>1074</v>
       </c>
-    </row>
-    <row r="168" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="P167" s="1">
+        <v>0</v>
+      </c>
+      <c r="Q167" s="1">
+        <v>0</v>
+      </c>
+      <c r="R167" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="168" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A168" s="1" t="s">
         <v>803</v>
       </c>
@@ -27580,8 +29095,17 @@
       <c r="O168" s="1" t="s">
         <v>1074</v>
       </c>
-    </row>
-    <row r="169" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="P168" s="1">
+        <v>0</v>
+      </c>
+      <c r="Q168" s="1">
+        <v>0</v>
+      </c>
+      <c r="R168" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="169" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A169" s="1" t="s">
         <v>804</v>
       </c>
@@ -27624,8 +29148,17 @@
       <c r="O169" s="1" t="s">
         <v>1074</v>
       </c>
-    </row>
-    <row r="170" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="P169" s="1">
+        <v>0</v>
+      </c>
+      <c r="Q169" s="1">
+        <v>0</v>
+      </c>
+      <c r="R169" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="170" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A170" s="1" t="s">
         <v>805</v>
       </c>
@@ -27668,8 +29201,17 @@
       <c r="O170" s="1" t="s">
         <v>1074</v>
       </c>
-    </row>
-    <row r="171" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="P170" s="1">
+        <v>0</v>
+      </c>
+      <c r="Q170" s="1">
+        <v>0</v>
+      </c>
+      <c r="R170" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="171" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A171" s="1" t="s">
         <v>806</v>
       </c>
@@ -27712,8 +29254,17 @@
       <c r="O171" s="1" t="s">
         <v>1074</v>
       </c>
-    </row>
-    <row r="172" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="P171" s="1">
+        <v>0</v>
+      </c>
+      <c r="Q171" s="1">
+        <v>0</v>
+      </c>
+      <c r="R171" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="172" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A172" s="1" t="s">
         <v>807</v>
       </c>
@@ -27756,8 +29307,17 @@
       <c r="O172" s="1" t="s">
         <v>1074</v>
       </c>
-    </row>
-    <row r="173" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="P172" s="1">
+        <v>0</v>
+      </c>
+      <c r="Q172" s="1">
+        <v>0</v>
+      </c>
+      <c r="R172" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="173" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A173" s="1" t="s">
         <v>808</v>
       </c>
@@ -27800,8 +29360,17 @@
       <c r="O173" s="1" t="s">
         <v>1074</v>
       </c>
-    </row>
-    <row r="174" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="P173" s="1">
+        <v>0</v>
+      </c>
+      <c r="Q173" s="1">
+        <v>0</v>
+      </c>
+      <c r="R173" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="174" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A174" s="1" t="s">
         <v>809</v>
       </c>
@@ -27844,8 +29413,17 @@
       <c r="O174" s="1" t="s">
         <v>1074</v>
       </c>
-    </row>
-    <row r="175" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="P174" s="1">
+        <v>0</v>
+      </c>
+      <c r="Q174" s="1">
+        <v>0</v>
+      </c>
+      <c r="R174" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="175" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A175" s="1" t="s">
         <v>810</v>
       </c>
@@ -27888,8 +29466,17 @@
       <c r="O175" s="1" t="s">
         <v>1074</v>
       </c>
-    </row>
-    <row r="176" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="P175" s="1">
+        <v>0</v>
+      </c>
+      <c r="Q175" s="1">
+        <v>0</v>
+      </c>
+      <c r="R175" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="176" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A176" s="1" t="s">
         <v>811</v>
       </c>
@@ -27932,8 +29519,17 @@
       <c r="O176" s="1" t="s">
         <v>1074</v>
       </c>
-    </row>
-    <row r="177" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="P176" s="1">
+        <v>0</v>
+      </c>
+      <c r="Q176" s="1">
+        <v>0</v>
+      </c>
+      <c r="R176" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="177" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A177" s="1" t="s">
         <v>812</v>
       </c>
@@ -27976,8 +29572,17 @@
       <c r="O177" s="1" t="s">
         <v>1074</v>
       </c>
-    </row>
-    <row r="178" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="P177" s="1">
+        <v>0</v>
+      </c>
+      <c r="Q177" s="1">
+        <v>0</v>
+      </c>
+      <c r="R177" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="178" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A178" s="1" t="s">
         <v>813</v>
       </c>
@@ -28020,8 +29625,17 @@
       <c r="O178" s="1" t="s">
         <v>1074</v>
       </c>
-    </row>
-    <row r="179" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="P178" s="1">
+        <v>0</v>
+      </c>
+      <c r="Q178" s="1">
+        <v>0</v>
+      </c>
+      <c r="R178" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="179" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A179" s="1" t="s">
         <v>814</v>
       </c>
@@ -28064,8 +29678,17 @@
       <c r="O179" s="1" t="s">
         <v>1074</v>
       </c>
-    </row>
-    <row r="180" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="P179" s="1">
+        <v>0</v>
+      </c>
+      <c r="Q179" s="1">
+        <v>0</v>
+      </c>
+      <c r="R179" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="180" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A180" s="1" t="s">
         <v>815</v>
       </c>
@@ -28108,8 +29731,17 @@
       <c r="O180" s="1" t="s">
         <v>1074</v>
       </c>
-    </row>
-    <row r="181" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="P180" s="1">
+        <v>0</v>
+      </c>
+      <c r="Q180" s="1">
+        <v>0</v>
+      </c>
+      <c r="R180" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="181" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A181" s="1" t="s">
         <v>816</v>
       </c>
@@ -28152,8 +29784,17 @@
       <c r="O181" s="1" t="s">
         <v>1074</v>
       </c>
-    </row>
-    <row r="182" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="P181" s="1">
+        <v>0</v>
+      </c>
+      <c r="Q181" s="1">
+        <v>0</v>
+      </c>
+      <c r="R181" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="182" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A182" s="1" t="s">
         <v>817</v>
       </c>
@@ -28196,8 +29837,17 @@
       <c r="O182" s="1" t="s">
         <v>1074</v>
       </c>
-    </row>
-    <row r="183" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="P182" s="1">
+        <v>0</v>
+      </c>
+      <c r="Q182" s="1">
+        <v>0</v>
+      </c>
+      <c r="R182" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="183" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A183" s="1" t="s">
         <v>818</v>
       </c>
@@ -28240,8 +29890,17 @@
       <c r="O183" s="1" t="s">
         <v>1074</v>
       </c>
-    </row>
-    <row r="184" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="P183" s="1">
+        <v>0</v>
+      </c>
+      <c r="Q183" s="1">
+        <v>0</v>
+      </c>
+      <c r="R183" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="184" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A184" s="1" t="s">
         <v>819</v>
       </c>
@@ -28283,6 +29942,15 @@
       </c>
       <c r="O184" s="1" t="s">
         <v>1074</v>
+      </c>
+      <c r="P184" s="1">
+        <v>0</v>
+      </c>
+      <c r="Q184" s="1">
+        <v>0</v>
+      </c>
+      <c r="R184" s="1">
+        <v>0</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
feat: Improve chromVAR, GimmeMotifs and SuSiE process
</commit_message>
<xml_diff>
--- a/scATAC/data/sample.xlsx
+++ b/scATAC/data/sample.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\software\JetBrains\JetBrains\PyCharm\PyCharmwp\scvdb_reproducibility\scATAC\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{87B948AA-CBA6-4457-A631-132469C75655}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EF782203-AAF9-48C2-868D-207DA15893C6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20087,8 +20087,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8787CBC2-21FC-4588-B485-8742706CBCF3}">
   <dimension ref="A1:R184"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E24" sqref="E24"/>
+    <sheetView tabSelected="1" topLeftCell="A58" workbookViewId="0">
+      <selection activeCell="E60" sqref="E60"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -20096,7 +20096,7 @@
     <col min="1" max="1" width="13.75" style="1" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="10.875" style="1" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="9.625" style="1" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="15.75" style="1" customWidth="1"/>
+    <col min="4" max="4" width="14.75" style="1" customWidth="1"/>
     <col min="5" max="5" width="25.5" style="1" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="10.875" style="1" customWidth="1"/>
     <col min="7" max="7" width="10.625" style="1" customWidth="1"/>
@@ -24011,10 +24011,10 @@
         <v>1</v>
       </c>
       <c r="Q72" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="R72" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="73" spans="1:18" x14ac:dyDescent="0.2">
@@ -24064,10 +24064,10 @@
         <v>1</v>
       </c>
       <c r="Q73" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="R73" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="74" spans="1:18" x14ac:dyDescent="0.2">
@@ -24117,10 +24117,10 @@
         <v>1</v>
       </c>
       <c r="Q74" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="R74" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="75" spans="1:18" x14ac:dyDescent="0.2">
@@ -24170,10 +24170,10 @@
         <v>1</v>
       </c>
       <c r="Q75" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="R75" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="76" spans="1:18" x14ac:dyDescent="0.2">
@@ -24223,10 +24223,10 @@
         <v>1</v>
       </c>
       <c r="Q76" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="R76" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="77" spans="1:18" x14ac:dyDescent="0.2">

</xml_diff>

<commit_message>
feat: Improve age/sex/drug and SuSiE process
</commit_message>
<xml_diff>
--- a/scATAC/data/sample.xlsx
+++ b/scATAC/data/sample.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\software\JetBrains\JetBrains\PyCharm\PyCharmwp\scvdb_reproducibility\scATAC\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2D92CFC3-7FFC-4602-B01E-215FFDE85544}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AC8C7304-5A2C-4C30-A74F-647FB6493BE3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20088,7 +20088,7 @@
   <dimension ref="A1:R184"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="Q3" sqref="Q3"/>
+      <selection activeCell="P12" sqref="P12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>

</xml_diff>

<commit_message>
feat: Improved V2G differences in age, gender, and drug resistance
</commit_message>
<xml_diff>
--- a/scATAC/data/sample.xlsx
+++ b/scATAC/data/sample.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\software\JetBrains\JetBrains\PyCharm\PyCharmwp\scvdb_reproducibility\scATAC\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AC8C7304-5A2C-4C30-A74F-647FB6493BE3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9124ADF1-DA5F-4662-8686-26B54750AE65}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7329" uniqueCount="1091">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7329" uniqueCount="1092">
   <si>
     <t>gse_id</t>
   </si>
@@ -3631,6 +3631,10 @@
   </si>
   <si>
     <t>f_drug</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>sample_id_84</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -20087,8 +20091,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8787CBC2-21FC-4588-B485-8742706CBCF3}">
   <dimension ref="A1:R184"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="P12" sqref="P12"/>
+    <sheetView tabSelected="1" topLeftCell="A62" workbookViewId="0">
+      <selection activeCell="S85" sqref="S85"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -24655,7 +24659,7 @@
     </row>
     <row r="85" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A85" s="1" t="s">
-        <v>720</v>
+        <v>1091</v>
       </c>
       <c r="B85" s="1" t="s">
         <v>137</v>

</xml_diff>